<commit_message>
Selenium second commit and push
</commit_message>
<xml_diff>
--- a/src/test/java/Book1.xlsx
+++ b/src/test/java/Book1.xlsx
@@ -4,52 +4,76 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="108" windowWidth="22980" windowHeight="9288"/>
+    <workbookView xWindow="0" yWindow="2448" windowWidth="19116" windowHeight="4956"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Product Name</t>
-  </si>
-  <si>
-    <t>Product Price</t>
-  </si>
-  <si>
-    <t>samsung</t>
-  </si>
-  <si>
-    <t>vivo</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>iphone</t>
   </si>
   <si>
-    <t>Nothing</t>
-  </si>
-  <si>
     <t>redmi</t>
   </si>
   <si>
     <t>nokia</t>
+  </si>
+  <si>
+    <t>samsung234@mail.com</t>
+  </si>
+  <si>
+    <t>biswa234</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>passward</t>
+  </si>
+  <si>
+    <t>vivo2343@gmail.com</t>
+  </si>
+  <si>
+    <t>viv023444</t>
+  </si>
+  <si>
+    <t>Nothing2323@gmail.com</t>
+  </si>
+  <si>
+    <t>bhohf345</t>
+  </si>
+  <si>
+    <t>balia456@gmail.com</t>
+  </si>
+  <si>
+    <t>bhibu567</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -72,13 +96,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -378,73 +405,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>26000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>4</v>
       </c>
       <c r="B4">
         <v>99000</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>5</v>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="B5">
         <v>40000</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B6">
         <v>30000</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B7">
         <v>25000</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8260539737</v>
+      </c>
+      <c r="B10">
+        <v>9861000762</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A5" r:id="rId3"/>
+    <hyperlink ref="A9" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>